<commit_message>
Apartado 3: criterios de comparación. FINALIZADO
</commit_message>
<xml_diff>
--- a/RepartoTG2 (1).xlsx
+++ b/RepartoTG2 (1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cheda\Documents\Cheda\Sistemas de Información\3º SISTEMAS DE INFORMACIÓN\SEGUNDO CUATRIMESTRE\DTE\LAB\TG2_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FDFF04-832E-4618-A057-D1299E261023}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>1) Autores, planificación, entrega</t>
   </si>
@@ -65,19 +66,25 @@
     <t>Urbano</t>
   </si>
   <si>
-    <t>Fernando Criterios E y F</t>
-  </si>
-  <si>
     <t>Martina</t>
   </si>
   <si>
     <t>Martina y Alberto</t>
+  </si>
+  <si>
+    <t>José y Fernando</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>José, Fernando Criterios E y F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,20 +422,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.08984375" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -444,69 +451,71 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>